<commit_message>
new if nInd > 1000 save simulation results in bunches parallelisation (use same structurs and functions) of Individual simulation and Population simulation
</commit_message>
<xml_diff>
--- a/test/test_NO4/prepareInput/Workflow.xlsx
+++ b/test/test_NO4/prepareInput/Workflow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="468" windowWidth="19464" windowHeight="7620"/>
+    <workbookView xWindow="480" yWindow="468" windowWidth="19464" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="121">
   <si>
     <t>Code Identifier</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>Organism|PeripheralVenousBlood|Hydroxy_Itraconazole|Plasma (Peripheral Venous Blood)</t>
+  </si>
+  <si>
+    <t>Organism|Bone|Intracellular|Midazolam|Concentration in container</t>
+  </si>
+  <si>
+    <t>Output 6</t>
+  </si>
+  <si>
+    <t>Midazolam Bone</t>
   </si>
 </sst>
 </file>
@@ -813,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1124,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1144,7 @@
     <col min="2" max="2" width="39.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1157,8 +1166,11 @@
       <c r="G1" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>61</v>
       </c>
@@ -1180,8 +1192,11 @@
       <c r="G2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -1203,8 +1218,11 @@
       <c r="G3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>64</v>
       </c>
@@ -1226,8 +1244,11 @@
       <c r="G4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>42</v>
       </c>
@@ -1235,7 +1256,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>68</v>
       </c>
@@ -1257,8 +1278,11 @@
       <c r="G6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>71</v>
@@ -1268,8 +1292,9 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>72</v>
       </c>
@@ -1291,8 +1316,11 @@
       <c r="G8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>72</v>
       </c>
@@ -1314,8 +1342,11 @@
       <c r="G9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>72</v>
       </c>
@@ -1337,8 +1368,11 @@
       <c r="G10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>72</v>
       </c>
@@ -1360,8 +1394,11 @@
       <c r="G11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>72</v>
       </c>
@@ -1383,8 +1420,11 @@
       <c r="G12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>72</v>
       </c>
@@ -1406,8 +1446,11 @@
       <c r="G13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>72</v>
       </c>
@@ -1429,8 +1472,11 @@
       <c r="G14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>72</v>
       </c>
@@ -1452,8 +1498,11 @@
       <c r="G15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>72</v>
       </c>
@@ -1475,8 +1524,11 @@
       <c r="G16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>72</v>
       </c>
@@ -1498,8 +1550,11 @@
       <c r="G17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>72</v>
       </c>
@@ -1521,8 +1576,11 @@
       <c r="G18" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>72</v>
       </c>
@@ -1544,8 +1602,11 @@
       <c r="G19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>72</v>
       </c>
@@ -1567,8 +1628,11 @@
       <c r="G20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>72</v>
       </c>
@@ -1590,8 +1654,11 @@
       <c r="G21" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>72</v>
       </c>
@@ -1613,8 +1680,11 @@
       <c r="G22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>72</v>
       </c>
@@ -1636,8 +1706,11 @@
       <c r="G23" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>72</v>
       </c>
@@ -1659,8 +1732,11 @@
       <c r="G24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>72</v>
       </c>
@@ -1682,8 +1758,11 @@
       <c r="G25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>72</v>
       </c>
@@ -1705,8 +1784,11 @@
       <c r="G26" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>72</v>
       </c>
@@ -1728,8 +1810,11 @@
       <c r="G27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>72</v>
       </c>
@@ -1751,8 +1836,11 @@
       <c r="G28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>72</v>
       </c>
@@ -1774,8 +1862,11 @@
       <c r="G29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>72</v>
       </c>
@@ -1797,8 +1888,11 @@
       <c r="G30">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>72</v>
       </c>
@@ -1820,8 +1914,11 @@
       <c r="G31">
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>72</v>
       </c>
@@ -1843,8 +1940,11 @@
       <c r="G32">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>72</v>
       </c>
@@ -1866,8 +1966,11 @@
       <c r="G33">
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>72</v>
       </c>
@@ -1887,6 +1990,9 @@
         <v>-1</v>
       </c>
       <c r="G34">
+        <v>-1</v>
+      </c>
+      <c r="H34">
         <v>-1</v>
       </c>
     </row>

</xml_diff>